<commit_message>
update T23 test case to reflect extra testing done by mentor on Mac and MacBook
</commit_message>
<xml_diff>
--- a/documentation/matrix 1.xlsx
+++ b/documentation/matrix 1.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -96,13 +95,6 @@
   </si>
   <si>
     <t>UX - Responsiveness</t>
-  </si>
-  <si>
-    <t>Repeat all above tests for desktop, tablet and smartphone screens sizes.  
-a. Laptop 1920 x 1080
-b. Tablet 768 x 1024 
-c. Larger tablet 1024 x 1366
-d. Smartphone 360 x 640</t>
   </si>
   <si>
     <t>F11 - End of Round screen</t>
@@ -497,6 +489,15 @@
 d. Text feedback message is visible on screen.
 e. Score of correct answers is visible on screen.
 f. "Play Again" and "End Game" buttons are visible and clickable on screen. </t>
+  </si>
+  <si>
+    <t>Repeat all above tests for desktop, tablet and smartphone screens sizes.  
+a. Laptop 1920 x 1080
+b. Tablet 768 x 1024 
+c. Larger tablet 1024 x 1366
+d. Smartphone 360 x 640
+e. iMac Pro 5120 x 2880
+f. 16" MacBook Pro 3072 x 1920</t>
   </si>
 </sst>
 </file>
@@ -1102,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>0</v>
@@ -1120,7 +1121,7 @@
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="19"/>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1138,7 +1139,7 @@
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="19"/>
       <c r="B6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
@@ -1156,7 +1157,7 @@
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1174,7 +1175,7 @@
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="19"/>
       <c r="B8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1192,7 +1193,7 @@
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="19"/>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1210,7 +1211,7 @@
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="19"/>
       <c r="B10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -1228,7 +1229,7 @@
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="19"/>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1248,7 +1249,7 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="19"/>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -1266,7 +1267,7 @@
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="19"/>
       <c r="B13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -1284,7 +1285,7 @@
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -1313,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1333,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>3</v>
@@ -1353,19 +1354,19 @@
         <v>9</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="13" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1373,19 +1374,19 @@
         <v>10</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="F3" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="13" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1393,19 +1394,19 @@
         <v>11</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:7" s="13" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,19 +1414,19 @@
         <v>12</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="13" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1433,19 +1434,19 @@
         <v>13</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="2:7" s="13" customFormat="1" ht="22.5" x14ac:dyDescent="0.2">
@@ -1453,19 +1454,19 @@
         <v>14</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="13" customFormat="1" ht="171" customHeight="1" x14ac:dyDescent="0.2">
@@ -1473,19 +1474,19 @@
         <v>15</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="F8" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="2:7" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1493,19 +1494,19 @@
         <v>16</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="2:7" s="13" customFormat="1" ht="78" customHeight="1" x14ac:dyDescent="0.2">
@@ -1513,19 +1514,19 @@
         <v>17</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>72</v>
-      </c>
       <c r="F10" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:7" s="13" customFormat="1" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1533,19 +1534,19 @@
         <v>18</v>
       </c>
       <c r="C11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>74</v>
-      </c>
       <c r="E11" s="12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:7" s="13" customFormat="1" ht="147" customHeight="1" x14ac:dyDescent="0.2">
@@ -1553,19 +1554,19 @@
         <v>19</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="E12" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>77</v>
-      </c>
       <c r="F12" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="2:7" s="13" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.2">
@@ -1573,19 +1574,19 @@
         <v>20</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:7" s="13" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -1593,19 +1594,19 @@
         <v>21</v>
       </c>
       <c r="C14" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="E14" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>81</v>
-      </c>
       <c r="F14" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="2:7" s="13" customFormat="1" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1613,19 +1614,19 @@
         <v>22</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="F15" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="2:7" s="13" customFormat="1" ht="97.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1633,170 +1634,170 @@
         <v>23</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="F16" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="2:7" s="13" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B17" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:7" s="13" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B18" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:7" s="13" customFormat="1" ht="292.5" x14ac:dyDescent="0.2">
       <c r="B19" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>107</v>
-      </c>
       <c r="F19" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="2:7" s="13" customFormat="1" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:7" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B21" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>55</v>
-      </c>
       <c r="F21" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="2:7" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:7" s="13" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="13" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="12" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" s="13" customFormat="1" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>25</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>26</v>
+        <v>110</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>8</v>
@@ -1805,7 +1806,7 @@
         <v>24</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>